<commit_message>
added sales page and its route
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,7 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09db7156b42a7194/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_0FA7EF5802F4597437B67C7F80B9A74D3063A41C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49786AE0-7FEF-4DD0-9C44-C2E5557C84B4}"/>
+  <bookViews>
+    <workbookView xWindow="1104" yWindow="180" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="medicine" sheetId="1" r:id="rId1"/>
     <sheet name="distributor" sheetId="2" r:id="rId2"/>
@@ -9,37 +19,141 @@
     <sheet name="sales" sheetId="4" r:id="rId4"/>
     <sheet name="stock" sheetId="5" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Maker</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Dolo 650</t>
+  </si>
+  <si>
+    <t>Micro Labs</t>
+  </si>
+  <si>
+    <t>Paracetamol</t>
+  </si>
+  <si>
+    <t>Brufen</t>
+  </si>
+  <si>
+    <t>Abbott</t>
+  </si>
+  <si>
+    <t>Ibuprofen</t>
+  </si>
+  <si>
+    <t>Amoxil</t>
+  </si>
+  <si>
+    <t>GSK</t>
+  </si>
+  <si>
+    <t>Amoxicillin</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>jsijo</t>
+  </si>
+  <si>
+    <t>okosko</t>
+  </si>
+  <si>
+    <t>98789</t>
+  </si>
+  <si>
+    <t>ni098</t>
+  </si>
+  <si>
+    <t>jsojj@mail.ocm</t>
+  </si>
+  <si>
+    <t>djoijsd</t>
+  </si>
+  <si>
+    <t>Distributor</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>dsnosj</t>
+  </si>
+  <si>
+    <t>odskas</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>3929</t>
+  </si>
+  <si>
+    <t>Medicine_Name</t>
+  </si>
+  <si>
+    <t>Quantity_Sold</t>
+  </si>
+  <si>
+    <t>Sale_Price</t>
+  </si>
+  <si>
+    <t>Tatal_Amount</t>
+  </si>
+  <si>
+    <t>Sale_Date</t>
+  </si>
+  <si>
+    <t>aslkkdl</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>1211</t>
+  </si>
+  <si>
+    <t>102000</t>
+  </si>
+  <si>
+    <t>3220-04-12</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,13 +183,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,181 +522,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Maker</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Salt</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Dolo 650</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Micro Labs</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Paracetamol</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Brufen</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Abbott</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Ibuprofen</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Amoxil</v>
-      </c>
-      <c r="B4" t="str">
-        <v>GSK</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Amoxicillin</v>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError sqref="A1:C4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Company</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Contact</v>
-      </c>
-      <c r="D1" t="str">
-        <v>GST</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Email</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Website</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>jsijo</v>
-      </c>
-      <c r="B2" t="str">
-        <v>okosko</v>
-      </c>
-      <c r="C2" t="str">
-        <v>98789</v>
-      </c>
-      <c r="D2" t="str">
-        <v>ni098</v>
-      </c>
-      <c r="E2" t="str">
-        <v>jsojj@mail.ocm</v>
-      </c>
-      <c r="F2" t="str">
-        <v>djoijsd</v>
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Distributor</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Item</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Quantity</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Price</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>dsnosj</v>
-      </c>
-      <c r="B2" t="str">
-        <v>odskas</v>
-      </c>
-      <c r="C2" t="str">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="str">
-        <v>3929</v>
+      <c r="D2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError sqref="A1:D2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.8984375" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" customWidth="1"/>
+    <col min="5" max="5" width="11.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added stock page and its route
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,7 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09db7156b42a7194/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_4DB6A6C006E572D43F795C5802C898A577B69E36" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A052B35-F0DA-4BEA-A2DD-C47FC51505D5}"/>
+  <bookViews>
+    <workbookView xWindow="1104" yWindow="180" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="medicine" sheetId="1" r:id="rId1"/>
     <sheet name="distributor" sheetId="2" r:id="rId2"/>
@@ -9,37 +19,165 @@
     <sheet name="sales" sheetId="4" r:id="rId4"/>
     <sheet name="stock" sheetId="5" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Maker</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Dolo 650</t>
+  </si>
+  <si>
+    <t>Micro Labs</t>
+  </si>
+  <si>
+    <t>Paracetamol</t>
+  </si>
+  <si>
+    <t>Brufen</t>
+  </si>
+  <si>
+    <t>Abbott</t>
+  </si>
+  <si>
+    <t>Ibuprofen</t>
+  </si>
+  <si>
+    <t>Amoxil</t>
+  </si>
+  <si>
+    <t>GSK</t>
+  </si>
+  <si>
+    <t>Amoxicillin</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>jsijo</t>
+  </si>
+  <si>
+    <t>okosko</t>
+  </si>
+  <si>
+    <t>98789</t>
+  </si>
+  <si>
+    <t>ni098</t>
+  </si>
+  <si>
+    <t>jsojj@mail.ocm</t>
+  </si>
+  <si>
+    <t>djoijsd</t>
+  </si>
+  <si>
+    <t>Distributor</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>dsnosj</t>
+  </si>
+  <si>
+    <t>odskas</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>3929</t>
+  </si>
+  <si>
+    <t>Medicine_Name</t>
+  </si>
+  <si>
+    <t>Quantity_Sold</t>
+  </si>
+  <si>
+    <t>Sale_Price</t>
+  </si>
+  <si>
+    <t>Tatal_Amount</t>
+  </si>
+  <si>
+    <t>Sale_Date</t>
+  </si>
+  <si>
+    <t>aslkkdl</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>1211</t>
+  </si>
+  <si>
+    <t>102000</t>
+  </si>
+  <si>
+    <t>3220-04-12</t>
+  </si>
+  <si>
+    <t>Stock_Quantity</t>
+  </si>
+  <si>
+    <t>Purchase_Price</t>
+  </si>
+  <si>
+    <t>Expiry_Date</t>
+  </si>
+  <si>
+    <t>combiflam</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>2025-03-02</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,13 +207,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,181 +546,268 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Maker</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Salt</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Dolo 650</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Micro Labs</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Paracetamol</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Brufen</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Abbott</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Ibuprofen</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Amoxil</v>
-      </c>
-      <c r="B4" t="str">
-        <v>GSK</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Amoxicillin</v>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError sqref="A1:C4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Company</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Contact</v>
-      </c>
-      <c r="D1" t="str">
-        <v>GST</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Email</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Website</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>jsijo</v>
-      </c>
-      <c r="B2" t="str">
-        <v>okosko</v>
-      </c>
-      <c r="C2" t="str">
-        <v>98789</v>
-      </c>
-      <c r="D2" t="str">
-        <v>ni098</v>
-      </c>
-      <c r="E2" t="str">
-        <v>jsojj@mail.ocm</v>
-      </c>
-      <c r="F2" t="str">
-        <v>djoijsd</v>
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Distributor</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Item</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Quantity</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Price</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>dsnosj</v>
-      </c>
-      <c r="B2" t="str">
-        <v>odskas</v>
-      </c>
-      <c r="C2" t="str">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="str">
-        <v>3929</v>
+      <c r="D2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError sqref="A1:D2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.09765625" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="15.296875" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated excel file and added in public
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09db7156b42a7194/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_4DB6A6C006E572D43F795C5802C898A577B69E36" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A052B35-F0DA-4BEA-A2DD-C47FC51505D5}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_5F72686638448E88CE362A27E9420CA3410848EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91DC69FE-F182-423F-8A19-B94DCCA65FF3}"/>
   <bookViews>
-    <workbookView xWindow="1104" yWindow="180" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1104" yWindow="180" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="medicine" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -35,31 +38,31 @@
     <t>Salt</t>
   </si>
   <si>
-    <t>Dolo 650</t>
-  </si>
-  <si>
-    <t>Micro Labs</t>
-  </si>
-  <si>
-    <t>Paracetamol</t>
-  </si>
-  <si>
-    <t>Brufen</t>
-  </si>
-  <si>
-    <t>Abbott</t>
-  </si>
-  <si>
-    <t>Ibuprofen</t>
-  </si>
-  <si>
-    <t>Amoxil</t>
-  </si>
-  <si>
-    <t>GSK</t>
-  </si>
-  <si>
-    <t>Amoxicillin</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>BatchNo</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>mmmm</t>
+  </si>
+  <si>
+    <t>cccc</t>
+  </si>
+  <si>
+    <t>ssss</t>
+  </si>
+  <si>
+    <t>pain killer</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>2025-03-21</t>
   </si>
   <si>
     <t>Company</t>
@@ -95,10 +98,10 @@
     <t>djoijsd</t>
   </si>
   <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>Item</t>
+    <t>DistributorID</t>
+  </si>
+  <si>
+    <t>MedicineID</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -107,16 +110,19 @@
     <t>Price</t>
   </si>
   <si>
-    <t>dsnosj</t>
-  </si>
-  <si>
-    <t>odskas</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>3929</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>2023-11-02</t>
   </si>
   <si>
     <t>Medicine_Name</t>
@@ -134,19 +140,16 @@
     <t>Sale_Date</t>
   </si>
   <si>
-    <t>aslkkdl</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>1211</t>
-  </si>
-  <si>
-    <t>102000</t>
-  </si>
-  <si>
-    <t>3220-04-12</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>2027-03-02</t>
   </si>
   <si>
     <t>Stock_Quantity</t>
@@ -158,19 +161,19 @@
     <t>Expiry_Date</t>
   </si>
   <si>
-    <t>combiflam</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>2025-03-02</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>2020-03-04</t>
   </si>
 </sst>
 </file>
@@ -547,13 +550,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,50 +566,114 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F2" t="s">
         <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:G2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -618,39 +685,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -661,135 +728,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.296875" customWidth="1"/>
+    <col min="2" max="2" width="10.296875" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" customWidth="1"/>
+    <col min="7" max="7" width="10.8984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D2" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.09765625" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="15.296875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="14.69921875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
@@ -802,12 +839,15 @@
       </c>
       <c r="E2" t="s">
         <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
slightly polished db structure change in excel
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09db7156b42a7194/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_5F72686638448E88CE362A27E9420CA3410848EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91DC69FE-F182-423F-8A19-B94DCCA65FF3}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_6E2AD3832DA77F0CBE38A60A413DBFE57D7A2949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D44839A3-7AE1-4A8B-9BA0-983F53B4452A}"/>
   <bookViews>
-    <workbookView xWindow="1104" yWindow="180" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="156" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="medicine" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -32,6 +32,39 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>jsijo</t>
+  </si>
+  <si>
+    <t>okosko</t>
+  </si>
+  <si>
+    <t>98789</t>
+  </si>
+  <si>
+    <t>ni098</t>
+  </si>
+  <si>
+    <t>jsojj@mail.ocm</t>
+  </si>
+  <si>
+    <t>djoijsd</t>
+  </si>
+  <si>
     <t>Maker</t>
   </si>
   <si>
@@ -65,45 +98,18 @@
     <t>2025-03-21</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>GST</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>jsijo</t>
-  </si>
-  <si>
-    <t>okosko</t>
-  </si>
-  <si>
-    <t>98789</t>
-  </si>
-  <si>
-    <t>ni098</t>
-  </si>
-  <si>
-    <t>jsojj@mail.ocm</t>
-  </si>
-  <si>
-    <t>djoijsd</t>
-  </si>
-  <si>
     <t>DistributorID</t>
   </si>
   <si>
     <t>MedicineID</t>
   </si>
   <si>
+    <t>Distributor_Name</t>
+  </si>
+  <si>
+    <t>Medicine_Name</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -116,16 +122,13 @@
     <t>1</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>2023-11-02</t>
-  </si>
-  <si>
-    <t>Medicine_Name</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>2024-04-03</t>
   </si>
   <si>
     <t>Quantity_Sold</t>
@@ -140,40 +143,28 @@
     <t>Sale_Date</t>
   </si>
   <si>
-    <t>12</t>
+    <t>150</t>
+  </si>
+  <si>
+    <t>2022-09-08</t>
+  </si>
+  <si>
+    <t>Stock_Quantity</t>
+  </si>
+  <si>
+    <t>Purchase_Price</t>
+  </si>
+  <si>
+    <t>Expiry_Date</t>
   </si>
   <si>
     <t>1200</t>
   </si>
   <si>
-    <t>15000</t>
-  </si>
-  <si>
-    <t>2027-03-02</t>
-  </si>
-  <si>
-    <t>Stock_Quantity</t>
-  </si>
-  <si>
-    <t>Purchase_Price</t>
-  </si>
-  <si>
-    <t>Expiry_Date</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>2020-03-04</t>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>2021-09-03</t>
   </si>
 </sst>
 </file>
@@ -674,13 +665,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,31 +690,43 @@
       <c r="F1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -732,15 +735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.296875" customWidth="1"/>
-    <col min="2" max="2" width="10.296875" customWidth="1"/>
-    <col min="6" max="6" width="11.59765625" customWidth="1"/>
-    <col min="7" max="7" width="10.8984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -750,19 +747,19 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -770,22 +767,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
       <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
         <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -798,13 +795,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="16.09765625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -812,42 +819,48 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>